<commit_message>
fraud order clustering updated
</commit_message>
<xml_diff>
--- a/models/cluster_centroids.xlsx
+++ b/models/cluster_centroids.xlsx
@@ -429,51 +429,51 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>0.7854506867240533</v>
+        <v>-0.6543059420995511</v>
       </c>
       <c r="B2">
-        <v>-0.594013903316271</v>
+        <v>-0.3750265906033246</v>
       </c>
       <c r="C2">
-        <v>-0.02056617296411334</v>
+        <v>-0.0211677942505568</v>
       </c>
       <c r="D2">
-        <v>-0.2835972681023712</v>
+        <v>-0.3170477670292229</v>
       </c>
       <c r="E2">
-        <v>-6.106226635438361E-16</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>1.387778780781446E-17</v>
+        <v>-2.081668171172169E-17</v>
       </c>
       <c r="G2">
-        <v>-5.828670879282072E-16</v>
+        <v>0.9999999999999994</v>
       </c>
       <c r="H2">
-        <v>0.9999999999999991</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>0.7854506867240543</v>
+        <v>0.7854506867240532</v>
       </c>
       <c r="B3">
-        <v>1.293650268947062</v>
+        <v>-0.7737767544714674</v>
       </c>
       <c r="C3">
-        <v>0.18807198116547</v>
+        <v>-0.07186316574642991</v>
       </c>
       <c r="D3">
-        <v>-0.6139127014755381</v>
+        <v>-0.1354182099528265</v>
       </c>
       <c r="E3">
-        <v>-5.828670879282072E-16</v>
+        <v>-5.551115123125783E-16</v>
       </c>
       <c r="F3">
-        <v>4.163336342344337E-17</v>
+        <v>6.938893903907228E-18</v>
       </c>
       <c r="G3">
-        <v>-5.273559366969494E-16</v>
+        <v>-4.996003610813204E-16</v>
       </c>
       <c r="H3">
         <v>0.9999999999999991</v>
@@ -481,129 +481,129 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>0.1884784259923157</v>
+        <v>0.7854506867240538</v>
       </c>
       <c r="B4">
-        <v>-0.7457021494381483</v>
+        <v>1.662784526844159</v>
       </c>
       <c r="C4">
-        <v>-2.007881171872831</v>
+        <v>0.2690051516089162</v>
       </c>
       <c r="D4">
-        <v>1.190963295584529</v>
+        <v>-0.6144788000646805</v>
       </c>
       <c r="E4">
-        <v>0.1788617886178862</v>
+        <v>-4.440892098500626E-16</v>
       </c>
       <c r="F4">
-        <v>0.01626016260162601</v>
+        <v>2.081668171172169E-17</v>
       </c>
       <c r="G4">
-        <v>0.1138211382113821</v>
+        <v>-4.163336342344337E-16</v>
       </c>
       <c r="H4">
-        <v>0.6910569105691057</v>
+        <v>0.9999999999999993</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
-        <v>-0.6543059420995507</v>
+        <v>-1.171595550543004</v>
       </c>
       <c r="B5">
-        <v>-0.5937811564221598</v>
+        <v>1.645333720546989</v>
       </c>
       <c r="C5">
-        <v>-0.05721873030293845</v>
+        <v>0.178767850818411</v>
       </c>
       <c r="D5">
-        <v>-0.2552164785910135</v>
+        <v>-0.6278761650676552</v>
       </c>
       <c r="E5">
-        <v>8.326672684688674E-17</v>
+        <v>0.37431693989071</v>
       </c>
       <c r="F5">
-        <v>-6.938893903907228E-18</v>
+        <v>0.1721311475409836</v>
       </c>
       <c r="G5">
-        <v>0.9999999999999993</v>
+        <v>0.453551912568306</v>
       </c>
       <c r="H5">
-        <v>1.110223024625157E-16</v>
+        <v>-1.110223024625157E-16</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6">
-        <v>0.01882702722057638</v>
+        <v>0.7854506867240526</v>
       </c>
       <c r="B6">
-        <v>0.2218143689568187</v>
+        <v>-0.7737767544714665</v>
       </c>
       <c r="C6">
-        <v>-4.827915638740398</v>
+        <v>0.5846248644017549</v>
       </c>
       <c r="D6">
-        <v>0.4663192749808097</v>
+        <v>1.558278797103807</v>
       </c>
       <c r="E6">
-        <v>0.1298701298701299</v>
+        <v>-2.775557561562891E-17</v>
       </c>
       <c r="F6">
-        <v>0.06493506493506493</v>
+        <v>-4.163336342344337E-17</v>
       </c>
       <c r="G6">
-        <v>0.2077922077922078</v>
+        <v>-2.775557561562891E-17</v>
       </c>
       <c r="H6">
-        <v>0.5974025974025974</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7">
-        <v>-1.541196025454888</v>
+        <v>-0.09092291342944422</v>
       </c>
       <c r="B7">
-        <v>-0.3538705019091366</v>
+        <v>-0.2082565583003272</v>
       </c>
       <c r="C7">
-        <v>-0.06221091009663797</v>
+        <v>-3.844752304992307</v>
       </c>
       <c r="D7">
-        <v>-0.3199538426099341</v>
+        <v>0.869652953261342</v>
       </c>
       <c r="E7">
-        <v>0.767999999999999</v>
+        <v>0.2028985507246377</v>
       </c>
       <c r="F7">
-        <v>0.232</v>
+        <v>0.05072463768115941</v>
       </c>
       <c r="G7">
-        <v>-1.665334536937735E-16</v>
+        <v>0.2028985507246377</v>
       </c>
       <c r="H7">
-        <v>-5.551115123125783E-16</v>
+        <v>0.5434782608695652</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8">
-        <v>-1.079762114437312</v>
+        <v>-1.152094138235371</v>
       </c>
       <c r="B8">
-        <v>1.461087984180791</v>
+        <v>-0.7737767544714664</v>
       </c>
       <c r="C8">
-        <v>0.1762622114793456</v>
+        <v>0.6345179914485616</v>
       </c>
       <c r="D8">
-        <v>-0.6222701534988139</v>
+        <v>1.568645793539876</v>
       </c>
       <c r="E8">
-        <v>0.3078651685393255</v>
+        <v>0.4574468085106378</v>
       </c>
       <c r="F8">
-        <v>0.1415730337078652</v>
+        <v>0.1170212765957447</v>
       </c>
       <c r="G8">
-        <v>0.5505617977528088</v>
+        <v>0.425531914893617</v>
       </c>
       <c r="H8">
         <v>-1.110223024625157E-16</v>
@@ -611,80 +611,80 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9">
-        <v>-1.155422648598225</v>
+        <v>0.1310158554405974</v>
       </c>
       <c r="B9">
-        <v>-0.7737767544714665</v>
+        <v>-0.7737767544714661</v>
       </c>
       <c r="C9">
-        <v>0.6295117886872502</v>
+        <v>3.360236373088318</v>
       </c>
       <c r="D9">
-        <v>1.564569390167711</v>
+        <v>9.660375904916965</v>
       </c>
       <c r="E9">
-        <v>0.4628975265017662</v>
+        <v>0.1818181818181818</v>
       </c>
       <c r="F9">
-        <v>0.1166077738515901</v>
+        <v>-6.938893903907228E-18</v>
       </c>
       <c r="G9">
-        <v>0.4204946996466431</v>
+        <v>0.1818181818181818</v>
       </c>
       <c r="H9">
-        <v>-2.220446049250313E-16</v>
+        <v>0.6363636363636364</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10">
-        <v>0.1310158554405974</v>
+        <v>-1.539215648748048</v>
       </c>
       <c r="B10">
-        <v>-0.7737767544714661</v>
+        <v>-0.3588496274335911</v>
       </c>
       <c r="C10">
-        <v>3.360236373088317</v>
+        <v>-0.0787566772044142</v>
       </c>
       <c r="D10">
-        <v>9.660375904916965</v>
+        <v>-0.3029033886073004</v>
       </c>
       <c r="E10">
-        <v>0.1818181818181818</v>
+        <v>0.7707509881422914</v>
       </c>
       <c r="F10">
-        <v>-6.938893903907228E-18</v>
+        <v>0.2292490118577075</v>
       </c>
       <c r="G10">
-        <v>0.1818181818181818</v>
+        <v>-1.387778780781446E-16</v>
       </c>
       <c r="H10">
-        <v>0.6363636363636364</v>
+        <v>-4.440892098500626E-16</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11">
-        <v>0.7854506867240526</v>
+        <v>0.7854506867240523</v>
       </c>
       <c r="B11">
-        <v>-0.7737767544714665</v>
+        <v>0.2523799260974036</v>
       </c>
       <c r="C11">
-        <v>0.6678764269111656</v>
+        <v>-0.01326833349065712</v>
       </c>
       <c r="D11">
-        <v>1.537886228946693</v>
+        <v>-0.6133489484600654</v>
       </c>
       <c r="E11">
-        <v>2.775557561562891E-17</v>
+        <v>-1.110223024625157E-16</v>
       </c>
       <c r="F11">
-        <v>-2.775557561562891E-17</v>
+        <v>-6.938893903907228E-17</v>
       </c>
       <c r="G11">
-        <v>2.775557561562891E-17</v>
+        <v>-1.665334536937735E-16</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>